<commit_message>
test case excel sheet upload
</commit_message>
<xml_diff>
--- a/Assignment1_Template_TestCollateralReport (1) (2).xlsx
+++ b/Assignment1_Template_TestCollateralReport (1) (2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Conestoga\Teaching\3_2024May\PROG2070-1_ProgrammingSoftwareQualityAssurance\Assignments\Assignment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\Archi Chambial\Archi Chambial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB3A138-1808-4BAC-BB11-62F6EDB39E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369D4CCE-814C-4388-A0E3-FF7140457EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="871" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestExecutionSchedule-Sprint1" sheetId="19" r:id="rId1"/>
@@ -25,23 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="74">
   <si>
     <t>Test Execution Schedule</t>
   </si>
@@ -242,9 +231,6 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>BLOCKED</t>
-  </si>
-  <si>
     <t>Registration</t>
   </si>
   <si>
@@ -254,13 +240,19 @@
     <t>F1</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>XYZ</t>
-  </si>
-  <si>
     <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>chechk input</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>after registrtion acknowledge</t>
+  </si>
+  <si>
+    <t>after login acknowledge</t>
   </si>
 </sst>
 </file>
@@ -796,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -981,9 +973,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -996,19 +985,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1017,15 +997,6 @@
     <xf numFmtId="0" fontId="12" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1034,6 +1005,21 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1353,36 +1339,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6408C84-166D-40EF-9E8F-55B471335ADA}">
   <dimension ref="B2:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="25" style="22" customWidth="1"/>
-    <col min="6" max="7" width="14.33203125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" style="22" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" style="22" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.28515625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="22" customWidth="1"/>
     <col min="10" max="10" width="9" style="22"/>
-    <col min="11" max="11" width="12.109375" style="22" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="22" customWidth="1"/>
     <col min="12" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" thickBot="1">
       <c r="B3" s="30"/>
@@ -1395,11 +1381,11 @@
       <c r="I3" s="30"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" thickBot="1">
-      <c r="K4" s="76" t="s">
+      <c r="K4" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="77"/>
-      <c r="M4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="79"/>
     </row>
     <row r="5" spans="2:17" ht="24.75" customHeight="1">
       <c r="B5" s="31" t="s">
@@ -1479,18 +1465,18 @@
       <c r="I7" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="75"/>
+      <c r="L7" s="71"/>
       <c r="M7" s="53">
         <f>COUNTA(C6:C15)</f>
         <v>7</v>
       </c>
-      <c r="O7" s="79" t="s">
+      <c r="O7" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="P7" s="80"/>
+      <c r="P7" s="73"/>
       <c r="Q7" s="54">
         <f>M7</f>
         <v>7</v>
@@ -1519,18 +1505,18 @@
       <c r="I8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="74" t="s">
+      <c r="K8" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="75"/>
+      <c r="L8" s="71"/>
       <c r="M8" s="53">
         <f>COUNTIFS(D6:D14,"Pass")</f>
         <v>3</v>
       </c>
-      <c r="O8" s="79" t="s">
+      <c r="O8" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="81"/>
+      <c r="P8" s="74"/>
       <c r="Q8" s="55">
         <f>(M8/M7)</f>
         <v>0.42857142857142855</v>
@@ -1557,18 +1543,18 @@
       <c r="I9" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="74" t="s">
+      <c r="K9" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="75"/>
+      <c r="L9" s="71"/>
       <c r="M9" s="53">
         <f>COUNTIFS(D6:D14,"Fail")</f>
         <v>0</v>
       </c>
-      <c r="O9" s="79" t="s">
+      <c r="O9" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="81"/>
+      <c r="P9" s="74"/>
       <c r="Q9" s="55">
         <f>(M9/M7)</f>
         <v>0</v>
@@ -1595,18 +1581,18 @@
       <c r="I10" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="74" t="s">
+      <c r="K10" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="75"/>
+      <c r="L10" s="71"/>
       <c r="M10" s="53">
         <f>COUNTIFS(D6:D14,"Blocked")</f>
         <v>4</v>
       </c>
-      <c r="O10" s="79" t="s">
+      <c r="O10" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="80"/>
+      <c r="P10" s="73"/>
       <c r="Q10" s="55">
         <f>(M10/M7)</f>
         <v>0.5714285714285714</v>
@@ -1633,10 +1619,10 @@
       <c r="I11" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="74" t="s">
+      <c r="K11" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="75"/>
+      <c r="L11" s="71"/>
       <c r="M11" s="53">
         <f>COUNTA(E6:E14)</f>
         <v>1</v>
@@ -1702,17 +1688,17 @@
     <row r="30" ht="26.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I13" xr:uid="{8ECF7AA4-347E-4E14-800C-6C874734C945}">
@@ -1733,29 +1719,29 @@
   </sheetPr>
   <dimension ref="B1:O294"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="6" width="28.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="19.77734375" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1"/>
+    <col min="5" max="6" width="28.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="30.21875" customWidth="1"/>
-    <col min="14" max="14" width="11.88671875" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="14.4"/>
+    <row r="1" spans="2:15" ht="15"/>
     <row r="2" spans="2:15" ht="46.5" customHeight="1">
       <c r="B2" s="5" t="s">
         <v>36</v>
@@ -1768,7 +1754,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
@@ -1796,19 +1782,19 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="25.5" customHeight="1">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="79"/>
       <c r="N4" s="26" t="s">
         <v>43</v>
       </c>
@@ -1860,7 +1846,7 @@
       </c>
       <c r="N6"/>
     </row>
-    <row r="7" spans="2:15" s="4" customFormat="1" ht="69">
+    <row r="7" spans="2:15" s="4" customFormat="1" ht="71.25">
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1895,7 +1881,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:15" s="4" customFormat="1" ht="13.8">
+    <row r="8" spans="2:15" s="4" customFormat="1" ht="14.25">
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -1908,7 +1894,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="2:15" s="4" customFormat="1" ht="13.8">
+    <row r="9" spans="2:15" s="4" customFormat="1" ht="14.25">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13"/>
@@ -1921,7 +1907,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="23"/>
     </row>
-    <row r="10" spans="2:15" s="4" customFormat="1" ht="13.8">
+    <row r="10" spans="2:15" s="4" customFormat="1" ht="14.25">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -1934,7 +1920,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="2:15" s="4" customFormat="1" ht="13.8">
+    <row r="11" spans="2:15" s="4" customFormat="1" ht="14.25">
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1947,7 +1933,7 @@
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
     </row>
-    <row r="12" spans="2:15" s="4" customFormat="1" ht="17.399999999999999">
+    <row r="12" spans="2:15" s="4" customFormat="1" ht="18">
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1960,288 +1946,288 @@
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
     </row>
-    <row r="13" spans="2:15" s="3" customFormat="1" ht="14.4"/>
-    <row r="14" spans="2:15" s="3" customFormat="1" ht="14.4"/>
-    <row r="15" spans="2:15" s="3" customFormat="1" ht="14.4"/>
-    <row r="16" spans="2:15" s="3" customFormat="1" ht="14.4"/>
-    <row r="17" s="3" customFormat="1" ht="14.4"/>
-    <row r="18" s="3" customFormat="1" ht="14.4"/>
-    <row r="19" s="3" customFormat="1" ht="14.4"/>
-    <row r="20" s="3" customFormat="1" ht="14.4"/>
-    <row r="21" s="3" customFormat="1" ht="14.4"/>
-    <row r="22" s="3" customFormat="1" ht="14.4"/>
-    <row r="23" s="3" customFormat="1" ht="14.4"/>
-    <row r="24" s="3" customFormat="1" ht="14.4"/>
-    <row r="25" s="3" customFormat="1" ht="14.4"/>
-    <row r="26" s="3" customFormat="1" ht="14.4"/>
-    <row r="27" s="3" customFormat="1" ht="14.4"/>
-    <row r="28" s="3" customFormat="1" ht="14.4"/>
-    <row r="29" s="3" customFormat="1" ht="14.4"/>
-    <row r="30" s="3" customFormat="1" ht="14.4"/>
-    <row r="31" s="3" customFormat="1" ht="14.4"/>
-    <row r="32" s="3" customFormat="1" ht="14.4"/>
-    <row r="33" s="3" customFormat="1" ht="14.4"/>
-    <row r="34" s="3" customFormat="1" ht="14.4"/>
-    <row r="35" s="3" customFormat="1" ht="14.4"/>
-    <row r="36" s="3" customFormat="1" ht="14.4"/>
-    <row r="37" s="3" customFormat="1" ht="14.4"/>
-    <row r="38" s="3" customFormat="1" ht="14.4"/>
-    <row r="39" s="3" customFormat="1" ht="14.4"/>
-    <row r="40" s="3" customFormat="1" ht="14.4"/>
-    <row r="41" s="3" customFormat="1" ht="14.4"/>
-    <row r="42" s="3" customFormat="1" ht="14.4"/>
-    <row r="43" s="3" customFormat="1" ht="14.4"/>
-    <row r="44" s="3" customFormat="1" ht="14.4"/>
-    <row r="45" s="3" customFormat="1" ht="14.4"/>
-    <row r="46" s="3" customFormat="1" ht="14.4"/>
-    <row r="47" s="3" customFormat="1" ht="14.4"/>
-    <row r="48" s="3" customFormat="1" ht="14.4"/>
-    <row r="49" s="3" customFormat="1" ht="14.4"/>
-    <row r="50" s="3" customFormat="1" ht="14.4"/>
-    <row r="51" s="3" customFormat="1" ht="14.4"/>
-    <row r="52" s="3" customFormat="1" ht="14.4"/>
-    <row r="53" s="3" customFormat="1" ht="14.4"/>
-    <row r="54" s="3" customFormat="1" ht="14.4"/>
-    <row r="55" s="3" customFormat="1" ht="14.4"/>
-    <row r="56" s="3" customFormat="1" ht="14.4"/>
-    <row r="57" s="3" customFormat="1" ht="14.4"/>
-    <row r="58" s="3" customFormat="1" ht="14.4"/>
-    <row r="59" s="3" customFormat="1" ht="14.4"/>
-    <row r="60" s="3" customFormat="1" ht="14.4"/>
-    <row r="61" s="3" customFormat="1" ht="14.4"/>
-    <row r="62" s="3" customFormat="1" ht="14.4"/>
-    <row r="63" s="3" customFormat="1" ht="14.4"/>
-    <row r="64" s="3" customFormat="1" ht="14.4"/>
-    <row r="65" s="3" customFormat="1" ht="14.4"/>
-    <row r="66" s="3" customFormat="1" ht="14.4"/>
-    <row r="67" s="3" customFormat="1" ht="14.4"/>
-    <row r="68" s="3" customFormat="1" ht="14.4"/>
-    <row r="69" s="3" customFormat="1" ht="14.4"/>
-    <row r="70" s="3" customFormat="1" ht="14.4"/>
-    <row r="71" s="3" customFormat="1" ht="14.4"/>
-    <row r="72" s="3" customFormat="1" ht="14.4"/>
-    <row r="73" s="3" customFormat="1" ht="14.4"/>
-    <row r="74" s="3" customFormat="1" ht="14.4"/>
-    <row r="75" s="3" customFormat="1" ht="14.4"/>
-    <row r="76" s="3" customFormat="1" ht="14.4"/>
-    <row r="77" s="3" customFormat="1" ht="14.4"/>
-    <row r="78" s="3" customFormat="1" ht="14.4"/>
-    <row r="79" s="3" customFormat="1" ht="14.4"/>
-    <row r="80" s="3" customFormat="1" ht="14.4"/>
-    <row r="81" s="3" customFormat="1" ht="14.4"/>
-    <row r="82" s="3" customFormat="1" ht="14.4"/>
-    <row r="83" s="3" customFormat="1" ht="14.4"/>
-    <row r="84" s="3" customFormat="1" ht="14.4"/>
-    <row r="85" s="3" customFormat="1" ht="14.4"/>
-    <row r="86" s="3" customFormat="1" ht="14.4"/>
-    <row r="87" s="3" customFormat="1" ht="14.4"/>
-    <row r="88" s="3" customFormat="1" ht="14.4"/>
-    <row r="89" s="3" customFormat="1" ht="14.4"/>
-    <row r="90" s="3" customFormat="1" ht="14.4"/>
-    <row r="91" s="3" customFormat="1" ht="14.4"/>
-    <row r="92" s="3" customFormat="1" ht="14.4"/>
-    <row r="93" s="3" customFormat="1" ht="14.4"/>
-    <row r="94" s="3" customFormat="1" ht="14.4"/>
-    <row r="95" s="3" customFormat="1" ht="14.4"/>
-    <row r="96" s="3" customFormat="1" ht="14.4"/>
-    <row r="97" s="3" customFormat="1" ht="14.4"/>
-    <row r="98" s="3" customFormat="1" ht="14.4"/>
-    <row r="99" s="3" customFormat="1" ht="14.4"/>
-    <row r="100" s="3" customFormat="1" ht="14.4"/>
-    <row r="101" s="3" customFormat="1" ht="14.4"/>
-    <row r="102" s="3" customFormat="1" ht="14.4"/>
-    <row r="103" s="3" customFormat="1" ht="14.4"/>
-    <row r="104" s="3" customFormat="1" ht="14.4"/>
-    <row r="105" s="3" customFormat="1" ht="14.4"/>
-    <row r="106" s="3" customFormat="1" ht="14.4"/>
-    <row r="107" s="3" customFormat="1" ht="14.4"/>
-    <row r="108" s="3" customFormat="1" ht="14.4"/>
-    <row r="109" s="3" customFormat="1" ht="14.4"/>
-    <row r="110" s="3" customFormat="1" ht="14.4"/>
-    <row r="111" s="3" customFormat="1" ht="14.4"/>
-    <row r="112" s="3" customFormat="1" ht="14.4"/>
-    <row r="113" s="3" customFormat="1" ht="14.4"/>
-    <row r="114" s="3" customFormat="1" ht="14.4"/>
-    <row r="115" s="3" customFormat="1" ht="14.4"/>
-    <row r="116" s="3" customFormat="1" ht="14.4"/>
-    <row r="117" s="3" customFormat="1" ht="14.4"/>
-    <row r="118" s="3" customFormat="1" ht="14.4"/>
-    <row r="119" s="3" customFormat="1" ht="14.4"/>
-    <row r="120" s="3" customFormat="1" ht="14.4"/>
-    <row r="121" s="3" customFormat="1" ht="14.4"/>
-    <row r="122" s="3" customFormat="1" ht="14.4"/>
-    <row r="123" s="3" customFormat="1" ht="14.4"/>
-    <row r="124" s="3" customFormat="1" ht="14.4"/>
-    <row r="125" s="3" customFormat="1" ht="14.4"/>
-    <row r="126" s="3" customFormat="1" ht="14.4"/>
-    <row r="127" s="3" customFormat="1" ht="14.4"/>
-    <row r="128" s="3" customFormat="1" ht="14.4"/>
-    <row r="129" s="3" customFormat="1" ht="14.4"/>
-    <row r="130" s="3" customFormat="1" ht="14.4"/>
-    <row r="131" s="3" customFormat="1" ht="14.4"/>
-    <row r="132" s="3" customFormat="1" ht="14.4"/>
-    <row r="133" s="3" customFormat="1" ht="14.4"/>
-    <row r="134" s="3" customFormat="1" ht="14.4"/>
-    <row r="135" s="3" customFormat="1" ht="14.4"/>
-    <row r="136" s="3" customFormat="1" ht="14.4"/>
-    <row r="137" s="3" customFormat="1" ht="14.4"/>
-    <row r="138" s="3" customFormat="1" ht="14.4"/>
-    <row r="139" s="3" customFormat="1" ht="14.4"/>
-    <row r="140" s="3" customFormat="1" ht="14.4"/>
-    <row r="141" s="3" customFormat="1" ht="14.4"/>
-    <row r="142" s="3" customFormat="1" ht="14.4"/>
-    <row r="143" s="3" customFormat="1" ht="14.4"/>
-    <row r="144" s="3" customFormat="1" ht="14.4"/>
-    <row r="145" s="3" customFormat="1" ht="14.4"/>
-    <row r="146" s="3" customFormat="1" ht="14.4"/>
-    <row r="147" s="3" customFormat="1" ht="14.4"/>
-    <row r="148" s="3" customFormat="1" ht="14.4"/>
-    <row r="149" s="3" customFormat="1" ht="14.4"/>
-    <row r="150" s="3" customFormat="1" ht="14.4"/>
-    <row r="151" s="3" customFormat="1" ht="14.4"/>
-    <row r="152" s="3" customFormat="1" ht="14.4"/>
-    <row r="153" s="3" customFormat="1" ht="14.4"/>
-    <row r="154" s="3" customFormat="1" ht="14.4"/>
-    <row r="155" s="3" customFormat="1" ht="14.4"/>
-    <row r="156" s="3" customFormat="1" ht="14.4"/>
-    <row r="157" s="3" customFormat="1" ht="14.4"/>
-    <row r="158" s="3" customFormat="1" ht="14.4"/>
-    <row r="159" s="3" customFormat="1" ht="14.4"/>
-    <row r="160" s="3" customFormat="1" ht="14.4"/>
-    <row r="161" s="3" customFormat="1" ht="14.4"/>
-    <row r="162" s="3" customFormat="1" ht="14.4"/>
-    <row r="163" s="3" customFormat="1" ht="14.4"/>
-    <row r="164" s="3" customFormat="1" ht="14.4"/>
-    <row r="165" s="3" customFormat="1" ht="14.4"/>
-    <row r="166" s="3" customFormat="1" ht="14.4"/>
-    <row r="167" s="3" customFormat="1" ht="14.4"/>
-    <row r="168" s="3" customFormat="1" ht="14.4"/>
-    <row r="169" s="3" customFormat="1" ht="14.4"/>
-    <row r="170" s="3" customFormat="1" ht="14.4"/>
-    <row r="171" s="3" customFormat="1" ht="14.4"/>
-    <row r="172" s="3" customFormat="1" ht="14.4"/>
-    <row r="173" s="3" customFormat="1" ht="14.4"/>
-    <row r="174" s="3" customFormat="1" ht="14.4"/>
-    <row r="175" s="3" customFormat="1" ht="14.4"/>
-    <row r="176" s="3" customFormat="1" ht="14.4"/>
-    <row r="177" s="3" customFormat="1" ht="14.4"/>
-    <row r="178" s="3" customFormat="1" ht="14.4"/>
-    <row r="179" s="3" customFormat="1" ht="14.4"/>
-    <row r="180" s="3" customFormat="1" ht="14.4"/>
-    <row r="181" s="3" customFormat="1" ht="14.4"/>
-    <row r="182" s="3" customFormat="1" ht="14.4"/>
-    <row r="183" s="3" customFormat="1" ht="14.4"/>
-    <row r="184" s="3" customFormat="1" ht="14.4"/>
-    <row r="185" s="3" customFormat="1" ht="14.4"/>
-    <row r="186" s="3" customFormat="1" ht="14.4"/>
-    <row r="187" s="3" customFormat="1" ht="14.4"/>
-    <row r="188" s="3" customFormat="1" ht="14.4"/>
-    <row r="189" s="3" customFormat="1" ht="14.4"/>
-    <row r="190" s="3" customFormat="1" ht="14.4"/>
-    <row r="191" s="3" customFormat="1" ht="14.4"/>
-    <row r="192" s="3" customFormat="1" ht="14.4"/>
-    <row r="193" s="3" customFormat="1" ht="14.4"/>
-    <row r="194" s="3" customFormat="1" ht="14.4"/>
-    <row r="195" s="3" customFormat="1" ht="14.4"/>
-    <row r="196" s="3" customFormat="1" ht="14.4"/>
-    <row r="197" s="3" customFormat="1" ht="14.4"/>
-    <row r="198" s="3" customFormat="1" ht="14.4"/>
-    <row r="199" s="3" customFormat="1" ht="14.4"/>
-    <row r="200" s="3" customFormat="1" ht="14.4"/>
-    <row r="201" s="3" customFormat="1" ht="14.4"/>
-    <row r="202" s="3" customFormat="1" ht="14.4"/>
-    <row r="203" s="3" customFormat="1" ht="14.4"/>
-    <row r="204" s="3" customFormat="1" ht="14.4"/>
-    <row r="205" s="3" customFormat="1" ht="14.4"/>
-    <row r="206" s="3" customFormat="1" ht="14.4"/>
-    <row r="207" s="3" customFormat="1" ht="14.4"/>
-    <row r="208" s="3" customFormat="1" ht="14.4"/>
-    <row r="209" s="3" customFormat="1" ht="14.4"/>
-    <row r="210" s="3" customFormat="1" ht="14.4"/>
-    <row r="211" s="3" customFormat="1" ht="14.4"/>
-    <row r="212" s="3" customFormat="1" ht="14.4"/>
-    <row r="213" s="3" customFormat="1" ht="14.4"/>
-    <row r="214" s="3" customFormat="1" ht="14.4"/>
-    <row r="215" s="3" customFormat="1" ht="14.4"/>
-    <row r="216" s="3" customFormat="1" ht="14.4"/>
-    <row r="217" s="3" customFormat="1" ht="14.4"/>
-    <row r="218" s="3" customFormat="1" ht="14.4"/>
-    <row r="219" s="3" customFormat="1" ht="14.4"/>
-    <row r="220" s="3" customFormat="1" ht="14.4"/>
-    <row r="221" s="3" customFormat="1" ht="14.4"/>
-    <row r="222" s="3" customFormat="1" ht="14.4"/>
-    <row r="223" s="3" customFormat="1" ht="14.4"/>
-    <row r="224" s="3" customFormat="1" ht="14.4"/>
-    <row r="225" s="3" customFormat="1" ht="14.4"/>
-    <row r="226" s="3" customFormat="1" ht="14.4"/>
-    <row r="227" s="3" customFormat="1" ht="14.4"/>
-    <row r="228" s="3" customFormat="1" ht="14.4"/>
-    <row r="229" s="3" customFormat="1" ht="14.4"/>
-    <row r="230" s="3" customFormat="1" ht="14.4"/>
-    <row r="231" s="3" customFormat="1" ht="14.4"/>
-    <row r="232" s="3" customFormat="1" ht="14.4"/>
-    <row r="233" s="3" customFormat="1" ht="14.4"/>
-    <row r="234" s="3" customFormat="1" ht="14.4"/>
-    <row r="235" s="3" customFormat="1" ht="14.4"/>
-    <row r="236" s="3" customFormat="1" ht="14.4"/>
-    <row r="237" s="3" customFormat="1" ht="14.4"/>
-    <row r="238" s="3" customFormat="1" ht="14.4"/>
-    <row r="239" s="3" customFormat="1" ht="14.4"/>
-    <row r="240" s="3" customFormat="1" ht="14.4"/>
-    <row r="241" s="3" customFormat="1" ht="14.4"/>
-    <row r="242" s="3" customFormat="1" ht="14.4"/>
-    <row r="243" s="3" customFormat="1" ht="14.4"/>
-    <row r="244" s="3" customFormat="1" ht="14.4"/>
-    <row r="245" s="3" customFormat="1" ht="14.4"/>
-    <row r="246" s="3" customFormat="1" ht="14.4"/>
-    <row r="247" s="3" customFormat="1" ht="14.4"/>
-    <row r="248" s="3" customFormat="1" ht="14.4"/>
-    <row r="249" s="3" customFormat="1" ht="14.4"/>
-    <row r="250" s="3" customFormat="1" ht="14.4"/>
-    <row r="251" s="3" customFormat="1" ht="14.4"/>
-    <row r="252" s="3" customFormat="1" ht="14.4"/>
-    <row r="253" s="3" customFormat="1" ht="14.4"/>
-    <row r="254" s="3" customFormat="1" ht="14.4"/>
-    <row r="255" s="3" customFormat="1" ht="14.4"/>
-    <row r="256" s="3" customFormat="1" ht="14.4"/>
-    <row r="257" s="3" customFormat="1" ht="14.4"/>
-    <row r="258" s="3" customFormat="1" ht="14.4"/>
-    <row r="259" s="3" customFormat="1" ht="14.4"/>
-    <row r="260" s="3" customFormat="1" ht="14.4"/>
-    <row r="261" s="3" customFormat="1" ht="14.4"/>
-    <row r="262" s="3" customFormat="1" ht="14.4"/>
-    <row r="263" s="3" customFormat="1" ht="14.4"/>
-    <row r="264" s="3" customFormat="1" ht="14.4"/>
-    <row r="265" s="3" customFormat="1" ht="14.4"/>
-    <row r="266" s="3" customFormat="1" ht="14.4"/>
-    <row r="267" s="3" customFormat="1" ht="14.4"/>
-    <row r="268" s="3" customFormat="1" ht="14.4"/>
-    <row r="269" s="3" customFormat="1" ht="14.4"/>
-    <row r="270" s="3" customFormat="1" ht="14.4"/>
-    <row r="271" s="3" customFormat="1" ht="14.4"/>
-    <row r="272" s="3" customFormat="1" ht="14.4"/>
-    <row r="273" s="3" customFormat="1" ht="14.4"/>
-    <row r="274" s="3" customFormat="1" ht="14.4"/>
-    <row r="275" s="3" customFormat="1" ht="14.4"/>
-    <row r="276" s="3" customFormat="1" ht="14.4"/>
-    <row r="277" s="3" customFormat="1" ht="14.4"/>
-    <row r="278" s="3" customFormat="1" ht="14.4"/>
-    <row r="279" s="3" customFormat="1" ht="14.4"/>
-    <row r="280" s="3" customFormat="1" ht="14.4"/>
-    <row r="281" s="3" customFormat="1" ht="14.4"/>
-    <row r="282" s="3" customFormat="1" ht="14.4"/>
-    <row r="283" s="3" customFormat="1" ht="14.4"/>
-    <row r="284" s="3" customFormat="1" ht="14.4"/>
-    <row r="285" s="3" customFormat="1" ht="14.4"/>
-    <row r="286" s="3" customFormat="1" ht="14.4"/>
-    <row r="287" s="3" customFormat="1" ht="14.4"/>
-    <row r="288" s="3" customFormat="1" ht="14.4"/>
-    <row r="289" s="3" customFormat="1" ht="14.4"/>
-    <row r="290" s="3" customFormat="1" ht="14.4"/>
-    <row r="291" s="3" customFormat="1" ht="14.4"/>
-    <row r="292" s="3" customFormat="1" ht="14.4"/>
-    <row r="293" s="3" customFormat="1" ht="14.4"/>
-    <row r="294" s="3" customFormat="1" ht="14.4"/>
+    <row r="13" spans="2:15" s="3" customFormat="1" ht="15"/>
+    <row r="14" spans="2:15" s="3" customFormat="1" ht="15"/>
+    <row r="15" spans="2:15" s="3" customFormat="1" ht="15"/>
+    <row r="16" spans="2:15" s="3" customFormat="1" ht="15"/>
+    <row r="17" s="3" customFormat="1" ht="15"/>
+    <row r="18" s="3" customFormat="1" ht="15"/>
+    <row r="19" s="3" customFormat="1" ht="15"/>
+    <row r="20" s="3" customFormat="1" ht="15"/>
+    <row r="21" s="3" customFormat="1" ht="15"/>
+    <row r="22" s="3" customFormat="1" ht="15"/>
+    <row r="23" s="3" customFormat="1" ht="15"/>
+    <row r="24" s="3" customFormat="1" ht="15"/>
+    <row r="25" s="3" customFormat="1" ht="15"/>
+    <row r="26" s="3" customFormat="1" ht="15"/>
+    <row r="27" s="3" customFormat="1" ht="15"/>
+    <row r="28" s="3" customFormat="1" ht="15"/>
+    <row r="29" s="3" customFormat="1" ht="15"/>
+    <row r="30" s="3" customFormat="1" ht="15"/>
+    <row r="31" s="3" customFormat="1" ht="15"/>
+    <row r="32" s="3" customFormat="1" ht="15"/>
+    <row r="33" s="3" customFormat="1" ht="15"/>
+    <row r="34" s="3" customFormat="1" ht="15"/>
+    <row r="35" s="3" customFormat="1" ht="15"/>
+    <row r="36" s="3" customFormat="1" ht="15"/>
+    <row r="37" s="3" customFormat="1" ht="15"/>
+    <row r="38" s="3" customFormat="1" ht="15"/>
+    <row r="39" s="3" customFormat="1" ht="15"/>
+    <row r="40" s="3" customFormat="1" ht="15"/>
+    <row r="41" s="3" customFormat="1" ht="15"/>
+    <row r="42" s="3" customFormat="1" ht="15"/>
+    <row r="43" s="3" customFormat="1" ht="15"/>
+    <row r="44" s="3" customFormat="1" ht="15"/>
+    <row r="45" s="3" customFormat="1" ht="15"/>
+    <row r="46" s="3" customFormat="1" ht="15"/>
+    <row r="47" s="3" customFormat="1" ht="15"/>
+    <row r="48" s="3" customFormat="1" ht="15"/>
+    <row r="49" s="3" customFormat="1" ht="15"/>
+    <row r="50" s="3" customFormat="1" ht="15"/>
+    <row r="51" s="3" customFormat="1" ht="15"/>
+    <row r="52" s="3" customFormat="1" ht="15"/>
+    <row r="53" s="3" customFormat="1" ht="15"/>
+    <row r="54" s="3" customFormat="1" ht="15"/>
+    <row r="55" s="3" customFormat="1" ht="15"/>
+    <row r="56" s="3" customFormat="1" ht="15"/>
+    <row r="57" s="3" customFormat="1" ht="15"/>
+    <row r="58" s="3" customFormat="1" ht="15"/>
+    <row r="59" s="3" customFormat="1" ht="15"/>
+    <row r="60" s="3" customFormat="1" ht="15"/>
+    <row r="61" s="3" customFormat="1" ht="15"/>
+    <row r="62" s="3" customFormat="1" ht="15"/>
+    <row r="63" s="3" customFormat="1" ht="15"/>
+    <row r="64" s="3" customFormat="1" ht="15"/>
+    <row r="65" s="3" customFormat="1" ht="15"/>
+    <row r="66" s="3" customFormat="1" ht="15"/>
+    <row r="67" s="3" customFormat="1" ht="15"/>
+    <row r="68" s="3" customFormat="1" ht="15"/>
+    <row r="69" s="3" customFormat="1" ht="15"/>
+    <row r="70" s="3" customFormat="1" ht="15"/>
+    <row r="71" s="3" customFormat="1" ht="15"/>
+    <row r="72" s="3" customFormat="1" ht="15"/>
+    <row r="73" s="3" customFormat="1" ht="15"/>
+    <row r="74" s="3" customFormat="1" ht="15"/>
+    <row r="75" s="3" customFormat="1" ht="15"/>
+    <row r="76" s="3" customFormat="1" ht="15"/>
+    <row r="77" s="3" customFormat="1" ht="15"/>
+    <row r="78" s="3" customFormat="1" ht="15"/>
+    <row r="79" s="3" customFormat="1" ht="15"/>
+    <row r="80" s="3" customFormat="1" ht="15"/>
+    <row r="81" s="3" customFormat="1" ht="15"/>
+    <row r="82" s="3" customFormat="1" ht="15"/>
+    <row r="83" s="3" customFormat="1" ht="15"/>
+    <row r="84" s="3" customFormat="1" ht="15"/>
+    <row r="85" s="3" customFormat="1" ht="15"/>
+    <row r="86" s="3" customFormat="1" ht="15"/>
+    <row r="87" s="3" customFormat="1" ht="15"/>
+    <row r="88" s="3" customFormat="1" ht="15"/>
+    <row r="89" s="3" customFormat="1" ht="15"/>
+    <row r="90" s="3" customFormat="1" ht="15"/>
+    <row r="91" s="3" customFormat="1" ht="15"/>
+    <row r="92" s="3" customFormat="1" ht="15"/>
+    <row r="93" s="3" customFormat="1" ht="15"/>
+    <row r="94" s="3" customFormat="1" ht="15"/>
+    <row r="95" s="3" customFormat="1" ht="15"/>
+    <row r="96" s="3" customFormat="1" ht="15"/>
+    <row r="97" s="3" customFormat="1" ht="15"/>
+    <row r="98" s="3" customFormat="1" ht="15"/>
+    <row r="99" s="3" customFormat="1" ht="15"/>
+    <row r="100" s="3" customFormat="1" ht="15"/>
+    <row r="101" s="3" customFormat="1" ht="15"/>
+    <row r="102" s="3" customFormat="1" ht="15"/>
+    <row r="103" s="3" customFormat="1" ht="15"/>
+    <row r="104" s="3" customFormat="1" ht="15"/>
+    <row r="105" s="3" customFormat="1" ht="15"/>
+    <row r="106" s="3" customFormat="1" ht="15"/>
+    <row r="107" s="3" customFormat="1" ht="15"/>
+    <row r="108" s="3" customFormat="1" ht="15"/>
+    <row r="109" s="3" customFormat="1" ht="15"/>
+    <row r="110" s="3" customFormat="1" ht="15"/>
+    <row r="111" s="3" customFormat="1" ht="15"/>
+    <row r="112" s="3" customFormat="1" ht="15"/>
+    <row r="113" s="3" customFormat="1" ht="15"/>
+    <row r="114" s="3" customFormat="1" ht="15"/>
+    <row r="115" s="3" customFormat="1" ht="15"/>
+    <row r="116" s="3" customFormat="1" ht="15"/>
+    <row r="117" s="3" customFormat="1" ht="15"/>
+    <row r="118" s="3" customFormat="1" ht="15"/>
+    <row r="119" s="3" customFormat="1" ht="15"/>
+    <row r="120" s="3" customFormat="1" ht="15"/>
+    <row r="121" s="3" customFormat="1" ht="15"/>
+    <row r="122" s="3" customFormat="1" ht="15"/>
+    <row r="123" s="3" customFormat="1" ht="15"/>
+    <row r="124" s="3" customFormat="1" ht="15"/>
+    <row r="125" s="3" customFormat="1" ht="15"/>
+    <row r="126" s="3" customFormat="1" ht="15"/>
+    <row r="127" s="3" customFormat="1" ht="15"/>
+    <row r="128" s="3" customFormat="1" ht="15"/>
+    <row r="129" s="3" customFormat="1" ht="15"/>
+    <row r="130" s="3" customFormat="1" ht="15"/>
+    <row r="131" s="3" customFormat="1" ht="15"/>
+    <row r="132" s="3" customFormat="1" ht="15"/>
+    <row r="133" s="3" customFormat="1" ht="15"/>
+    <row r="134" s="3" customFormat="1" ht="15"/>
+    <row r="135" s="3" customFormat="1" ht="15"/>
+    <row r="136" s="3" customFormat="1" ht="15"/>
+    <row r="137" s="3" customFormat="1" ht="15"/>
+    <row r="138" s="3" customFormat="1" ht="15"/>
+    <row r="139" s="3" customFormat="1" ht="15"/>
+    <row r="140" s="3" customFormat="1" ht="15"/>
+    <row r="141" s="3" customFormat="1" ht="15"/>
+    <row r="142" s="3" customFormat="1" ht="15"/>
+    <row r="143" s="3" customFormat="1" ht="15"/>
+    <row r="144" s="3" customFormat="1" ht="15"/>
+    <row r="145" s="3" customFormat="1" ht="15"/>
+    <row r="146" s="3" customFormat="1" ht="15"/>
+    <row r="147" s="3" customFormat="1" ht="15"/>
+    <row r="148" s="3" customFormat="1" ht="15"/>
+    <row r="149" s="3" customFormat="1" ht="15"/>
+    <row r="150" s="3" customFormat="1" ht="15"/>
+    <row r="151" s="3" customFormat="1" ht="15"/>
+    <row r="152" s="3" customFormat="1" ht="15"/>
+    <row r="153" s="3" customFormat="1" ht="15"/>
+    <row r="154" s="3" customFormat="1" ht="15"/>
+    <row r="155" s="3" customFormat="1" ht="15"/>
+    <row r="156" s="3" customFormat="1" ht="15"/>
+    <row r="157" s="3" customFormat="1" ht="15"/>
+    <row r="158" s="3" customFormat="1" ht="15"/>
+    <row r="159" s="3" customFormat="1" ht="15"/>
+    <row r="160" s="3" customFormat="1" ht="15"/>
+    <row r="161" s="3" customFormat="1" ht="15"/>
+    <row r="162" s="3" customFormat="1" ht="15"/>
+    <row r="163" s="3" customFormat="1" ht="15"/>
+    <row r="164" s="3" customFormat="1" ht="15"/>
+    <row r="165" s="3" customFormat="1" ht="15"/>
+    <row r="166" s="3" customFormat="1" ht="15"/>
+    <row r="167" s="3" customFormat="1" ht="15"/>
+    <row r="168" s="3" customFormat="1" ht="15"/>
+    <row r="169" s="3" customFormat="1" ht="15"/>
+    <row r="170" s="3" customFormat="1" ht="15"/>
+    <row r="171" s="3" customFormat="1" ht="15"/>
+    <row r="172" s="3" customFormat="1" ht="15"/>
+    <row r="173" s="3" customFormat="1" ht="15"/>
+    <row r="174" s="3" customFormat="1" ht="15"/>
+    <row r="175" s="3" customFormat="1" ht="15"/>
+    <row r="176" s="3" customFormat="1" ht="15"/>
+    <row r="177" s="3" customFormat="1" ht="15"/>
+    <row r="178" s="3" customFormat="1" ht="15"/>
+    <row r="179" s="3" customFormat="1" ht="15"/>
+    <row r="180" s="3" customFormat="1" ht="15"/>
+    <row r="181" s="3" customFormat="1" ht="15"/>
+    <row r="182" s="3" customFormat="1" ht="15"/>
+    <row r="183" s="3" customFormat="1" ht="15"/>
+    <row r="184" s="3" customFormat="1" ht="15"/>
+    <row r="185" s="3" customFormat="1" ht="15"/>
+    <row r="186" s="3" customFormat="1" ht="15"/>
+    <row r="187" s="3" customFormat="1" ht="15"/>
+    <row r="188" s="3" customFormat="1" ht="15"/>
+    <row r="189" s="3" customFormat="1" ht="15"/>
+    <row r="190" s="3" customFormat="1" ht="15"/>
+    <row r="191" s="3" customFormat="1" ht="15"/>
+    <row r="192" s="3" customFormat="1" ht="15"/>
+    <row r="193" s="3" customFormat="1" ht="15"/>
+    <row r="194" s="3" customFormat="1" ht="15"/>
+    <row r="195" s="3" customFormat="1" ht="15"/>
+    <row r="196" s="3" customFormat="1" ht="15"/>
+    <row r="197" s="3" customFormat="1" ht="15"/>
+    <row r="198" s="3" customFormat="1" ht="15"/>
+    <row r="199" s="3" customFormat="1" ht="15"/>
+    <row r="200" s="3" customFormat="1" ht="15"/>
+    <row r="201" s="3" customFormat="1" ht="15"/>
+    <row r="202" s="3" customFormat="1" ht="15"/>
+    <row r="203" s="3" customFormat="1" ht="15"/>
+    <row r="204" s="3" customFormat="1" ht="15"/>
+    <row r="205" s="3" customFormat="1" ht="15"/>
+    <row r="206" s="3" customFormat="1" ht="15"/>
+    <row r="207" s="3" customFormat="1" ht="15"/>
+    <row r="208" s="3" customFormat="1" ht="15"/>
+    <row r="209" s="3" customFormat="1" ht="15"/>
+    <row r="210" s="3" customFormat="1" ht="15"/>
+    <row r="211" s="3" customFormat="1" ht="15"/>
+    <row r="212" s="3" customFormat="1" ht="15"/>
+    <row r="213" s="3" customFormat="1" ht="15"/>
+    <row r="214" s="3" customFormat="1" ht="15"/>
+    <row r="215" s="3" customFormat="1" ht="15"/>
+    <row r="216" s="3" customFormat="1" ht="15"/>
+    <row r="217" s="3" customFormat="1" ht="15"/>
+    <row r="218" s="3" customFormat="1" ht="15"/>
+    <row r="219" s="3" customFormat="1" ht="15"/>
+    <row r="220" s="3" customFormat="1" ht="15"/>
+    <row r="221" s="3" customFormat="1" ht="15"/>
+    <row r="222" s="3" customFormat="1" ht="15"/>
+    <row r="223" s="3" customFormat="1" ht="15"/>
+    <row r="224" s="3" customFormat="1" ht="15"/>
+    <row r="225" s="3" customFormat="1" ht="15"/>
+    <row r="226" s="3" customFormat="1" ht="15"/>
+    <row r="227" s="3" customFormat="1" ht="15"/>
+    <row r="228" s="3" customFormat="1" ht="15"/>
+    <row r="229" s="3" customFormat="1" ht="15"/>
+    <row r="230" s="3" customFormat="1" ht="15"/>
+    <row r="231" s="3" customFormat="1" ht="15"/>
+    <row r="232" s="3" customFormat="1" ht="15"/>
+    <row r="233" s="3" customFormat="1" ht="15"/>
+    <row r="234" s="3" customFormat="1" ht="15"/>
+    <row r="235" s="3" customFormat="1" ht="15"/>
+    <row r="236" s="3" customFormat="1" ht="15"/>
+    <row r="237" s="3" customFormat="1" ht="15"/>
+    <row r="238" s="3" customFormat="1" ht="15"/>
+    <row r="239" s="3" customFormat="1" ht="15"/>
+    <row r="240" s="3" customFormat="1" ht="15"/>
+    <row r="241" s="3" customFormat="1" ht="15"/>
+    <row r="242" s="3" customFormat="1" ht="15"/>
+    <row r="243" s="3" customFormat="1" ht="15"/>
+    <row r="244" s="3" customFormat="1" ht="15"/>
+    <row r="245" s="3" customFormat="1" ht="15"/>
+    <row r="246" s="3" customFormat="1" ht="15"/>
+    <row r="247" s="3" customFormat="1" ht="15"/>
+    <row r="248" s="3" customFormat="1" ht="15"/>
+    <row r="249" s="3" customFormat="1" ht="15"/>
+    <row r="250" s="3" customFormat="1" ht="15"/>
+    <row r="251" s="3" customFormat="1" ht="15"/>
+    <row r="252" s="3" customFormat="1" ht="15"/>
+    <row r="253" s="3" customFormat="1" ht="15"/>
+    <row r="254" s="3" customFormat="1" ht="15"/>
+    <row r="255" s="3" customFormat="1" ht="15"/>
+    <row r="256" s="3" customFormat="1" ht="15"/>
+    <row r="257" s="3" customFormat="1" ht="15"/>
+    <row r="258" s="3" customFormat="1" ht="15"/>
+    <row r="259" s="3" customFormat="1" ht="15"/>
+    <row r="260" s="3" customFormat="1" ht="15"/>
+    <row r="261" s="3" customFormat="1" ht="15"/>
+    <row r="262" s="3" customFormat="1" ht="15"/>
+    <row r="263" s="3" customFormat="1" ht="15"/>
+    <row r="264" s="3" customFormat="1" ht="15"/>
+    <row r="265" s="3" customFormat="1" ht="15"/>
+    <row r="266" s="3" customFormat="1" ht="15"/>
+    <row r="267" s="3" customFormat="1" ht="15"/>
+    <row r="268" s="3" customFormat="1" ht="15"/>
+    <row r="269" s="3" customFormat="1" ht="15"/>
+    <row r="270" s="3" customFormat="1" ht="15"/>
+    <row r="271" s="3" customFormat="1" ht="15"/>
+    <row r="272" s="3" customFormat="1" ht="15"/>
+    <row r="273" s="3" customFormat="1" ht="15"/>
+    <row r="274" s="3" customFormat="1" ht="15"/>
+    <row r="275" s="3" customFormat="1" ht="15"/>
+    <row r="276" s="3" customFormat="1" ht="15"/>
+    <row r="277" s="3" customFormat="1" ht="15"/>
+    <row r="278" s="3" customFormat="1" ht="15"/>
+    <row r="279" s="3" customFormat="1" ht="15"/>
+    <row r="280" s="3" customFormat="1" ht="15"/>
+    <row r="281" s="3" customFormat="1" ht="15"/>
+    <row r="282" s="3" customFormat="1" ht="15"/>
+    <row r="283" s="3" customFormat="1" ht="15"/>
+    <row r="284" s="3" customFormat="1" ht="15"/>
+    <row r="285" s="3" customFormat="1" ht="15"/>
+    <row r="286" s="3" customFormat="1" ht="15"/>
+    <row r="287" s="3" customFormat="1" ht="15"/>
+    <row r="288" s="3" customFormat="1" ht="15"/>
+    <row r="289" s="3" customFormat="1" ht="15"/>
+    <row r="290" s="3" customFormat="1" ht="15"/>
+    <row r="291" s="3" customFormat="1" ht="15"/>
+    <row r="292" s="3" customFormat="1" ht="15"/>
+    <row r="293" s="3" customFormat="1" ht="15"/>
+    <row r="294" s="3" customFormat="1" ht="15"/>
   </sheetData>
   <autoFilter ref="B6:L7" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="0">
@@ -2262,40 +2248,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957244BA-1829-49AB-834C-A7E298367B0D}">
   <dimension ref="B1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" style="22" customWidth="1"/>
     <col min="5" max="5" width="25" style="22" customWidth="1"/>
-    <col min="6" max="7" width="14.33203125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" style="22" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" style="22" customWidth="1"/>
+    <col min="6" max="7" width="14.28515625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="22" customWidth="1"/>
     <col min="10" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="14.4" thickBot="1"/>
+    <row r="1" spans="2:13" ht="15" thickBot="1"/>
     <row r="2" spans="2:13" ht="15" customHeight="1" thickBot="1">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="K2" s="76" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="K2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="79"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1" thickBot="1">
       <c r="B3" s="30"/>
@@ -2327,7 +2313,7 @@
       <c r="D5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="65" t="s">
         <v>62</v>
       </c>
       <c r="F5" s="33" t="s">
@@ -2337,16 +2323,18 @@
         <v>7</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I5" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="K5" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="82"/>
-      <c r="M5" s="53"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="53">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="2:13" ht="27.75" customHeight="1" thickBot="1">
       <c r="B6" s="45" t="s">
@@ -2355,11 +2343,11 @@
       <c r="C6" s="46">
         <v>5</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="67" t="s">
-        <v>68</v>
+      <c r="E6" s="66" t="s">
+        <v>67</v>
       </c>
       <c r="F6" s="45">
         <v>1</v>
@@ -2367,15 +2355,19 @@
       <c r="G6" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="45"/>
-      <c r="I6" s="70" t="s">
+      <c r="H6" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="74" t="s">
+      <c r="K6" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="82"/>
-      <c r="M6" s="53"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="53">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:13" ht="27.75" customHeight="1" thickBot="1">
       <c r="B7" s="56" t="s">
@@ -2384,27 +2376,31 @@
       <c r="C7" s="50">
         <v>5</v>
       </c>
-      <c r="D7" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="56">
+      <c r="D7" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="45">
         <v>1</v>
       </c>
-      <c r="G7" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="K7" s="74" t="s">
+      <c r="G7" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="53"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="53">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="2:13" ht="30" customHeight="1" thickBot="1">
       <c r="B8" s="34" t="s">
@@ -2414,28 +2410,51 @@
         <v>1</v>
       </c>
       <c r="D8" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="56">
+        <v>1</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="34">
+      <c r="K8" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="80"/>
+      <c r="M8" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="30" customHeight="1">
+      <c r="D9" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="56">
         <v>1</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G9" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="K8" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="82"/>
-      <c r="M8" s="53"/>
-    </row>
-    <row r="9" spans="2:13" ht="30" customHeight="1"/>
+      <c r="H9" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="69" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="10" spans="2:13" ht="30" customHeight="1"/>
     <row r="11" spans="2:13" ht="30" customHeight="1"/>
     <row r="12" spans="2:13" ht="30" customHeight="1"/>
@@ -2460,7 +2479,7 @@
     <mergeCell ref="K7:L7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G8" xr:uid="{282CDF6E-DF76-40E2-B47A-B6C301E3DD18}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G9" xr:uid="{282CDF6E-DF76-40E2-B47A-B6C301E3DD18}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -2469,6 +2488,66 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ae49239-cb22-4cd7-a443-551e4e5c4d05" xsi:nil="true"/>
+    <SecondaryOwner_x002d_Ready_x003f_ xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">No</SecondaryOwner_x002d_Ready_x003f_>
+    <PrimaryOwner xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </PrimaryOwner>
+    <Tertiary xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Tertiary>
+    <HealthofDocument xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
+    <Effort_x0028_TshirtSize_x0029_ xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
+    <TertiaryOwner xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </TertiaryOwner>
+    <SecondaryOwner xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SecondaryOwner>
+    <EstimateofEffort xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
+    <SharedWithUsers xmlns="4ae49239-cb22-4cd7-a443-551e4e5c4d05">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100333322EE81FDC642BCEEB62E8BE8BAE1" ma:contentTypeVersion="27" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="59642bd4c7b6a76631958a5c52a67885">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="307604ce-6b0e-4d1c-bc76-6b04c545b021" xmlns:ns3="4ae49239-cb22-4cd7-a443-551e4e5c4d05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dda8fbd4595a4c129fc4d2718b60df1f" ns2:_="" ns3:_="">
     <xsd:import namespace="307604ce-6b0e-4d1c-bc76-6b04c545b021"/>
@@ -2840,67 +2919,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EAE76E1-1157-417E-A972-422E377D7DF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="307604ce-6b0e-4d1c-bc76-6b04c545b021"/>
+    <ds:schemaRef ds:uri="4ae49239-cb22-4cd7-a443-551e4e5c4d05"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ae49239-cb22-4cd7-a443-551e4e5c4d05" xsi:nil="true"/>
-    <SecondaryOwner_x002d_Ready_x003f_ xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">No</SecondaryOwner_x002d_Ready_x003f_>
-    <PrimaryOwner xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </PrimaryOwner>
-    <Tertiary xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Tertiary>
-    <HealthofDocument xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
-    <Effort_x0028_TshirtSize_x0029_ xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
-    <TertiaryOwner xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </TertiaryOwner>
-    <SecondaryOwner xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SecondaryOwner>
-    <EstimateofEffort xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
-    <SharedWithUsers xmlns="4ae49239-cb22-4cd7-a443-551e4e5c4d05">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="307604ce-6b0e-4d1c-bc76-6b04c545b021" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE0AD4A-3AAC-4F70-80C1-1675C086EA41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E228B387-3F6D-443C-8A29-A639589F7FF4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2917,23 +2955,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE0AD4A-3AAC-4F70-80C1-1675C086EA41}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EAE76E1-1157-417E-A972-422E377D7DF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="307604ce-6b0e-4d1c-bc76-6b04c545b021"/>
-    <ds:schemaRef ds:uri="4ae49239-cb22-4cd7-a443-551e4e5c4d05"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>